<commit_message>
correction definition extension b50f1b90109c520c243683b0c81f51ce1b96ecc5
</commit_message>
<xml_diff>
--- a/ig/sd-add-ext-consequences-principales-et-secondaires/StructureDefinition-eclaire-outcome-measure-r5.xlsx
+++ b/ig/sd-add-ext-consequences-principales-et-secondaires/StructureDefinition-eclaire-outcome-measure-r5.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-09T16:27:19+00:00</t>
+    <t>2024-02-09T16:53:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Extension créée dans le cadre du projet API ECLAIRE afin de permettre l'ajout de plusieurs titres pour l'essai. Cette extension implemente l'élément label de R5 https://hl7.org/fhir/researchstudy-definitions.html#ResearchStudy.label .</t>
+    <t>Extension créée dans le cadre du projet API ECLAIRE afin de permettre l'ajout ette extension implemente l'élément outcomeMeasure de R5. elle permet l'ajout des conséquences principales et secondaires de l'essai. Cette extension implemente l’élément outcomeMeasure de R5 http://hl7.org/fhir/R5/researchstudy-definitions.html#ResearchStudy.outcomeMeasure</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>